<commit_message>
draft schamatic & some documents
</commit_message>
<xml_diff>
--- a/doc/STM32F103xx-LQFP48 pin-out.xlsx
+++ b/doc/STM32F103xx-LQFP48 pin-out.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Variometer_STM32\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="11385"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="196">
   <si>
     <t>Pins</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -489,14 +494,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UART1_TX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UART1_RX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Remap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -537,18 +534,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SD_CS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EE_CS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC_POWER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JTMS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -565,10 +550,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LOW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BTN_RESET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -577,18 +558,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LED_STATE1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LED_STATE2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DISC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -761,10 +730,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Arduino Not Support</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SPI2_SCLK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -774,6 +739,46 @@
   </si>
   <si>
     <t>SPI2_MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_BATTERY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\SD_CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\EE_CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_MCU_STATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BT_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPS_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND(Pull-down to GND)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -893,9 +898,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -907,6 +909,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,7 +1185,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1190,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1213,37 +1218,37 @@
     <row r="3" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -1283,7 +1288,7 @@
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="6" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -1304,9 +1309,7 @@
         <v>17</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="J10" s="6" t="s">
-        <v>140</v>
-      </c>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
@@ -1380,7 +1383,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -1438,7 +1441,7 @@
       </c>
       <c r="H17" s="2"/>
       <c r="J17" s="7" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
@@ -1479,7 +1482,7 @@
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
@@ -1501,7 +1504,7 @@
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
@@ -1523,7 +1526,7 @@
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="7" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
@@ -1587,10 +1590,10 @@
         <v>35</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
@@ -1614,7 +1617,7 @@
         <v>37</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
@@ -1658,7 +1661,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="J27" s="8" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
@@ -1766,7 +1769,7 @@
       </c>
       <c r="H32" s="2"/>
       <c r="J32" s="6" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
@@ -1790,7 +1793,7 @@
       </c>
       <c r="H33" s="2"/>
       <c r="J33" s="7" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
@@ -1814,7 +1817,7 @@
       </c>
       <c r="H34" s="2"/>
       <c r="J34" s="6" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
@@ -1838,7 +1841,7 @@
       </c>
       <c r="H35" s="2"/>
       <c r="J35" s="6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
@@ -1862,7 +1865,7 @@
       </c>
       <c r="H36" s="2"/>
       <c r="J36" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
@@ -1886,7 +1889,7 @@
       </c>
       <c r="H37" s="2"/>
       <c r="J37" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
@@ -1910,7 +1913,7 @@
       </c>
       <c r="H38" s="2"/>
       <c r="J38" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
@@ -1918,7 +1921,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>20</v>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="H39" s="2"/>
       <c r="J39" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
@@ -1958,7 +1961,7 @@
       </c>
       <c r="H40" s="2"/>
       <c r="J40" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
@@ -1981,8 +1984,8 @@
       <c r="H41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="7" t="s">
-        <v>132</v>
+      <c r="J41" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
@@ -2114,7 +2117,7 @@
         <v>93</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
@@ -2138,7 +2141,7 @@
         <v>92</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.3">
@@ -2163,8 +2166,8 @@
       <c r="H49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J49" s="7" t="s">
-        <v>117</v>
+      <c r="J49" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="K49" s="6"/>
     </row>
@@ -2190,8 +2193,8 @@
       <c r="H50" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J50" s="7" t="s">
-        <v>118</v>
+      <c r="J50" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="K50" s="6"/>
     </row>
@@ -2212,7 +2215,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="J51" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
@@ -2237,8 +2240,8 @@
       <c r="H52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J52" s="5" t="s">
-        <v>126</v>
+      <c r="J52" s="7" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.3">
@@ -2263,8 +2266,8 @@
       <c r="H53" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J53" s="5" t="s">
-        <v>127</v>
+      <c r="J53" s="7" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.3">
@@ -2345,432 +2348,432 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>191</v>
+      <c r="C4" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>0</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="10">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="10">
+        <v>3</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="10">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="10">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="10">
+        <v>7</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="10">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="10">
+        <v>9</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="10">
+        <v>10</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="10">
+        <v>11</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="10">
+        <v>12</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="10">
+        <v>13</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="10">
+        <v>14</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="10">
+        <v>15</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="10">
+        <v>16</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="10">
+        <v>17</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="10">
+        <v>18</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="10">
+        <v>19</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="10">
+        <v>20</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="10">
+        <v>21</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="10">
+        <v>22</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="12" t="s">
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="10">
+        <v>23</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="12" t="s">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="10">
+        <v>24</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="11">
-        <v>2</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="11">
-        <v>3</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="11">
-        <v>4</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="11">
-        <v>5</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="11">
-        <v>6</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="11">
-        <v>7</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="11">
-        <v>8</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="11">
-        <v>9</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="11">
-        <v>10</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="11">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="11">
-        <v>12</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="11">
-        <v>13</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="11">
-        <v>14</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="11">
-        <v>15</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="11">
-        <v>16</v>
-      </c>
-      <c r="D22" s="12" t="s">
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="10">
+        <v>25</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="11">
-        <v>17</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="10">
+        <v>26</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="11">
-        <v>18</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="10">
+        <v>27</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="11">
-        <v>19</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="10">
+        <v>28</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="11">
-        <v>20</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="10">
+        <v>29</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="11">
-        <v>21</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="10">
+        <v>30</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="11">
-        <v>22</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="10">
+        <v>31</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="11">
-        <v>23</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="10">
+        <v>32</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="11">
-        <v>24</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="10">
+        <v>33</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="11">
-        <v>25</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="10">
+        <v>34</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="11">
-        <v>26</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="11">
-        <v>27</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="11">
-        <v>28</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="11">
-        <v>29</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="11">
-        <v>30</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="11">
-        <v>31</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="11">
-        <v>32</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="11">
-        <v>33</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="11">
-        <v>34</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
support auto power off
</commit_message>
<xml_diff>
--- a/doc/STM32F103xx-LQFP48 pin-out.xlsx
+++ b/doc/STM32F103xx-LQFP48 pin-out.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="198">
   <si>
     <t>Pins</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -779,6 +779,14 @@
   </si>
   <si>
     <t>remap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POWER_CTRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_DETECT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1195,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28:J29"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1317,9 @@
         <v>17</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
@@ -1640,7 +1650,9 @@
       <c r="H26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="6"/>
+      <c r="J26" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="2">

</xml_diff>

<commit_message>
calculate vertical velocity suppport ms5611 on stm32 some reference circuit & datasheet change pin map : eeprom -> i2c2, spi2 -> spi1, ...
</commit_message>
<xml_diff>
--- a/doc/STM32F103xx-LQFP48 pin-out.xlsx
+++ b/doc/STM32F103xx-LQFP48 pin-out.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Variometer_STM32\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="11385"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="238">
   <si>
     <t>Pins</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -787,6 +782,166 @@
   </si>
   <si>
     <t>USB_DETECT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EEPROM_SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EEPROM_SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD_CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD_SCLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD_MISO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD_MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POWER_CTRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART2_TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART2_Rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BATTERY_VOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USART1_RX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_DM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_DP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTCK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTDI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTDO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNTRST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN_CMD(BTN_BOOT)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C1_SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C1_SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BT_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPS_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM_H(TIM1_CH1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM_L(TIM1_CH1N)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND(Pull-Down to GND)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN_RESET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_MCU_STATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_DETECT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN_BOOT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -794,7 +949,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +969,52 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -875,7 +1076,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,6 +1121,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1193,7 +1424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1201,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K58"/>
+  <dimension ref="B1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1219,13 +1450,14 @@
     <col min="8" max="8" width="35.75" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="24.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1478,7 @@
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1259,7 +1491,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -1276,8 +1508,11 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>2</v>
       </c>
@@ -1298,8 +1533,11 @@
       <c r="J9" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>3</v>
       </c>
@@ -1320,8 +1558,11 @@
       <c r="J10" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>4</v>
       </c>
@@ -1339,8 +1580,11 @@
         <v>18</v>
       </c>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>5</v>
       </c>
@@ -1357,8 +1601,11 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>6</v>
       </c>
@@ -1375,8 +1622,11 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>7</v>
       </c>
@@ -1395,8 +1645,11 @@
       <c r="J14" s="8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>8</v>
       </c>
@@ -1413,8 +1666,11 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>9</v>
       </c>
@@ -1431,8 +1687,11 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>10</v>
       </c>
@@ -1453,8 +1712,11 @@
       <c r="J17" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>11</v>
       </c>
@@ -1472,8 +1734,11 @@
         <v>45</v>
       </c>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>12</v>
       </c>
@@ -1494,8 +1759,11 @@
       <c r="J19" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <v>13</v>
       </c>
@@ -1516,8 +1784,11 @@
       <c r="J20" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>14</v>
       </c>
@@ -1538,8 +1809,11 @@
       <c r="J21" s="7" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>15</v>
       </c>
@@ -1557,8 +1831,11 @@
         <v>41</v>
       </c>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
         <v>16</v>
       </c>
@@ -1578,8 +1855,11 @@
       <c r="H23" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>17</v>
       </c>
@@ -1599,14 +1879,17 @@
       <c r="H24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="17" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>18</v>
       </c>
@@ -1629,8 +1912,11 @@
       <c r="J25" s="7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>19</v>
       </c>
@@ -1653,8 +1939,11 @@
       <c r="J26" s="6" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>20</v>
       </c>
@@ -1675,8 +1964,11 @@
       <c r="J27" s="8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>21</v>
       </c>
@@ -1699,8 +1991,11 @@
         <v>33</v>
       </c>
       <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>22</v>
       </c>
@@ -1723,8 +2018,11 @@
         <v>59</v>
       </c>
       <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>23</v>
       </c>
@@ -1741,8 +2039,11 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>24</v>
       </c>
@@ -1759,8 +2060,11 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>25</v>
       </c>
@@ -1780,11 +2084,15 @@
         <v>114</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="23" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="21"/>
+      <c r="L32" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>26</v>
       </c>
@@ -1804,11 +2112,15 @@
         <v>60</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="J33" s="7" t="s">
+      <c r="J33" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="21"/>
+      <c r="L33" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>27</v>
       </c>
@@ -1831,8 +2143,11 @@
       <c r="J34" s="6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>28</v>
       </c>
@@ -1855,8 +2170,11 @@
       <c r="J35" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>29</v>
       </c>
@@ -1879,8 +2197,11 @@
       <c r="J36" s="7" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>30</v>
       </c>
@@ -1903,8 +2224,11 @@
       <c r="J37" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L37" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>31</v>
       </c>
@@ -1927,8 +2251,11 @@
       <c r="J38" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L38" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>32</v>
       </c>
@@ -1951,8 +2278,11 @@
       <c r="J39" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>33</v>
       </c>
@@ -1975,8 +2305,11 @@
       <c r="J40" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L40" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>34</v>
       </c>
@@ -1999,8 +2332,11 @@
       <c r="J41" s="9" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L41" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>35</v>
       </c>
@@ -2017,8 +2353,11 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L42" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>36</v>
       </c>
@@ -2035,8 +2374,11 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L43" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>37</v>
       </c>
@@ -2059,8 +2401,11 @@
       <c r="J44" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>38</v>
       </c>
@@ -2083,8 +2428,11 @@
       <c r="J45" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L45" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>39</v>
       </c>
@@ -2107,8 +2455,11 @@
       <c r="J46" s="9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L46" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>40</v>
       </c>
@@ -2131,8 +2482,11 @@
       <c r="J47" s="9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>41</v>
       </c>
@@ -2155,8 +2509,11 @@
       <c r="J48" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>42</v>
       </c>
@@ -2182,8 +2539,11 @@
         <v>124</v>
       </c>
       <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L49" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>43</v>
       </c>
@@ -2209,8 +2569,11 @@
         <v>125</v>
       </c>
       <c r="K50" s="6"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L50" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <v>44</v>
       </c>
@@ -2229,8 +2592,11 @@
       <c r="J51" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="2">
         <v>45</v>
       </c>
@@ -2255,8 +2621,11 @@
       <c r="J52" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>46</v>
       </c>
@@ -2281,8 +2650,11 @@
       <c r="J53" s="7" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L53" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>47</v>
       </c>
@@ -2299,8 +2671,11 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="J54" s="8"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="2">
         <v>48</v>
       </c>
@@ -2317,13 +2692,16 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="J55" s="8"/>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>111</v>
       </c>

</xml_diff>